<commit_message>
Add extra svg shapes
</commit_message>
<xml_diff>
--- a/resources/templates/template graaf input.xlsx
+++ b/resources/templates/template graaf input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beryl\Dropbox\prime\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf75de77b452b7ca/PRIME/prime-graaf/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01949122-2262-45A4-92DE-37142E55D483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="114_{F1254EB2-4834-4E57-A5B3-79A73A44A9E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{59EBEE8B-27E0-4152-9486-834F70E2E491}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1530" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Domains" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>Module</t>
   </si>
@@ -212,6 +212,18 @@
   </si>
   <si>
     <t>testcell</t>
+  </si>
+  <si>
+    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" preserveAspectRatio="none" viewBox="0 0 266.45 125.12"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#d6dded;stroke:#3255a4;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;Middel 1&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="subspaces"&gt;&lt;g id="node_kopie_18" data-name="node kopie 18"&gt;&lt;path class="cls-1" d="M240.52,123.12H27.65S-30.06,56.38,27.65,2H240.52C294.36,72.62,240.52,123.12,240.52,123.12Z"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
+  </si>
+  <si>
+    <t>#3255A4</t>
+  </si>
+  <si>
+    <t>&lt;svg xmlns="http://www.w3.org/2000/svg" preserveAspectRatio="none" viewBox="0 0 288.81 125.8"&gt;&lt;defs&gt;&lt;style&gt;.cls-1{fill:#dcf7e9;stroke:#50d691;stroke-miterlimit:10;stroke-width:4px;}&lt;/style&gt;&lt;/defs&gt;&lt;title&gt;Middel 3&lt;/title&gt;&lt;g id="Laag_2" data-name="Laag 2"&gt;&lt;g id="subspaces"&gt;&lt;g id="node_kopie_18" data-name="node kopie 18"&gt;&lt;path class="cls-1" d="M285.82,123.79l-282.71-.5s27.71-60.5,0-121.12c-.29-.38,282.71,0,282.71,0C260.82,62.79,285.82,123.79,285.82,123.79Z"/&gt;&lt;/g&gt;&lt;/g&gt;&lt;/g&gt;&lt;/svg&gt;</t>
+  </si>
+  <si>
+    <t>#50D691</t>
   </si>
 </sst>
 </file>
@@ -566,6 +578,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2514600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1261808</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Afbeelding 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B0F848E-6CC4-4E0B-97D5-1801D677AFAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3825240" y="7871461"/>
+          <a:ext cx="2529840" cy="1193227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>22861</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2522221</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1210906</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Afbeelding 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2947966-BC81-42F1-BBF2-1BFBED8767BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3863341" y="9380221"/>
+          <a:ext cx="2499360" cy="1096605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -868,17 +968,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -897,20 +997,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECFE40C-F157-443F-A97D-ABFBF3785C99}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="47.109375" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -922,7 +1022,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -930,7 +1030,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -938,7 +1038,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -946,7 +1046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -954,12 +1054,28 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -977,13 +1093,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -992,7 +1108,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1033,13 +1149,13 @@
       <selection activeCell="B1421" sqref="B1421"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1078,13 +1194,13 @@
       <selection activeCell="A1795" sqref="A1795"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1113,56 +1229,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AM30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="21" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="16" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1281,203 +1397,203 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C12"/>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
       <c r="G23"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
       <c r="C30"/>
       <c r="D30"/>
@@ -1511,9 +1627,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>